<commit_message>
WAITM-617 Update test file
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FF52FE-2906-4C47-99DB-7F76E3B1E6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FCE489-7EFF-E24D-BD1E-697D5B4D5976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="-18740" windowWidth="33100" windowHeight="16440" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>programCode</t>
   </si>
   <si>
-    <t>test-program</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -455,6 +452,9 @@
   </si>
   <si>
     <t>programs</t>
+  </si>
+  <si>
+    <t>test-questions-program</t>
   </si>
 </sst>
 </file>
@@ -818,7 +818,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,63 +842,63 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -906,22 +906,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>0</v>
@@ -956,187 +956,187 @@
   <sheetData>
     <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="P2" t="s">
         <v>132</v>
-      </c>
-      <c r="P2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K3" t="s">
+        <v>131</v>
+      </c>
+      <c r="P3" t="s">
         <v>132</v>
-      </c>
-      <c r="P3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" t="s">
         <v>132</v>
-      </c>
-      <c r="P4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1166,486 +1166,486 @@
   <sheetData>
     <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WAITM-617 Update unit tests
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FCE489-7EFF-E24D-BD1E-697D5B4D5976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007E2631-B1FC-0744-9C1C-22F5E7293E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="-18740" windowWidth="33100" windowHeight="16440" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
+    <workbookView xWindow="180" yWindow="-18740" windowWidth="33100" windowHeight="16440" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Question Validation Succeed" sheetId="3" r:id="rId2"/>
     <sheet name="Question Validation Fail" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -439,9 +439,6 @@
     <t>{ "unit": "kg" }</t>
   </si>
   <si>
-    <t>{ "column": "xyz", "writeToPatient": { "field": "abc", "isAdditionalData": false, "fieldType": "def" } }</t>
-  </si>
-  <si>
     <t>{ "column": "xyz" }</t>
   </si>
   <si>
@@ -455,6 +452,9 @@
   </si>
   <si>
     <t>test-questions-program</t>
+  </si>
+  <si>
+    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "def" } }</t>
   </si>
 </sst>
 </file>
@@ -817,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8F628F-AE1D-F84E-B5DC-4521B630F270}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -842,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -889,7 +889,7 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -912,7 +912,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,7 +1066,7 @@
         <v>125</v>
       </c>
       <c r="P5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1080,7 +1080,7 @@
         <v>126</v>
       </c>
       <c r="P6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -1094,7 +1094,7 @@
         <v>127</v>
       </c>
       <c r="P7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
         <v>128</v>
       </c>
       <c r="P8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -1122,7 +1122,7 @@
         <v>129</v>
       </c>
       <c r="P9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1136,7 +1136,7 @@
         <v>130</v>
       </c>
       <c r="P10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1148,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82512E0-EE41-F34F-B49B-D4799E578BC3}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B32"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
WAITM-617 Bugfixes, fixup testing errors (#3508)
* WAITM-617 Rounding as a number instead of a string

* WAITM-617 Update field to fieldName

* WAITM-617 Add "noUnknown" to nested objects

* WAITM-617 Add base config type to avoid unknown config fields

* WAITM-617 Make fieldType required

* WAITM-617 Add test to require "where" field _only_ if
source="ReferenceData"

* WAITM-617 Add scope to Autocomplete validation

* WAITM-617 Apply config schema to config

* WAITM-617 Update unit tests
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FCE489-7EFF-E24D-BD1E-697D5B4D5976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007E2631-B1FC-0744-9C1C-22F5E7293E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="-18740" windowWidth="33100" windowHeight="16440" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
+    <workbookView xWindow="180" yWindow="-18740" windowWidth="33100" windowHeight="16440" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Question Validation Succeed" sheetId="3" r:id="rId2"/>
     <sheet name="Question Validation Fail" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -439,9 +439,6 @@
     <t>{ "unit": "kg" }</t>
   </si>
   <si>
-    <t>{ "column": "xyz", "writeToPatient": { "field": "abc", "isAdditionalData": false, "fieldType": "def" } }</t>
-  </si>
-  <si>
     <t>{ "column": "xyz" }</t>
   </si>
   <si>
@@ -455,6 +452,9 @@
   </si>
   <si>
     <t>test-questions-program</t>
+  </si>
+  <si>
+    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "def" } }</t>
   </si>
 </sst>
 </file>
@@ -817,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8F628F-AE1D-F84E-B5DC-4521B630F270}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -842,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -889,7 +889,7 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -912,7 +912,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,7 +1066,7 @@
         <v>125</v>
       </c>
       <c r="P5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1080,7 +1080,7 @@
         <v>126</v>
       </c>
       <c r="P6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -1094,7 +1094,7 @@
         <v>127</v>
       </c>
       <c r="P7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
         <v>128</v>
       </c>
       <c r="P8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -1122,7 +1122,7 @@
         <v>129</v>
       </c>
       <c r="P9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -1136,7 +1136,7 @@
         <v>130</v>
       </c>
       <c r="P10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1148,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82512E0-EE41-F34F-B49B-D4799E578BC3}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B32"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Validate survey question calculation and writeToField.fieldType
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkennedy/proj/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007E2631-B1FC-0744-9C1C-22F5E7293E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD773F57-6DD4-3043-BEE2-F8EF30773747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="-18740" windowWidth="33100" windowHeight="16440" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
   <si>
     <t>programName</t>
   </si>
@@ -454,7 +454,13 @@
     <t>test-questions-program</t>
   </si>
   <si>
-    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "def" } }</t>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>2+2</t>
+  </si>
+  <si>
+    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "FreeText" } }</t>
   </si>
 </sst>
 </file>
@@ -473,6 +479,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -937,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1034,6 +1041,9 @@
       <c r="K3" t="s">
         <v>131</v>
       </c>
+      <c r="O3" t="s">
+        <v>138</v>
+      </c>
       <c r="P3" t="s">
         <v>132</v>
       </c>
@@ -1051,6 +1061,9 @@
       <c r="K4" t="s">
         <v>131</v>
       </c>
+      <c r="O4" t="s">
+        <v>139</v>
+      </c>
       <c r="P4" t="s">
         <v>132</v>
       </c>
@@ -1066,7 +1079,7 @@
         <v>125</v>
       </c>
       <c r="P5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1148,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82512E0-EE41-F34F-B49B-D4799E578BC3}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1283,6 +1296,9 @@
       <c r="K6" t="s">
         <v>105</v>
       </c>
+      <c r="O6" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1297,6 +1313,9 @@
       <c r="K7" t="s">
         <v>106</v>
       </c>
+      <c r="O7" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1308,6 +1327,9 @@
       <c r="C8" t="s">
         <v>67</v>
       </c>
+      <c r="O8" t="s">
+        <v>138</v>
+      </c>
       <c r="P8" t="s">
         <v>105</v>
       </c>
@@ -1322,6 +1344,9 @@
       <c r="C9" t="s">
         <v>68</v>
       </c>
+      <c r="O9" t="s">
+        <v>139</v>
+      </c>
       <c r="P9" t="s">
         <v>107</v>
       </c>
@@ -1339,6 +1364,9 @@
       <c r="K10" t="s">
         <v>105</v>
       </c>
+      <c r="O10" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1353,6 +1381,9 @@
       <c r="K11" t="s">
         <v>106</v>
       </c>
+      <c r="O11" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1364,6 +1395,9 @@
       <c r="C12" t="s">
         <v>71</v>
       </c>
+      <c r="O12" t="s">
+        <v>138</v>
+      </c>
       <c r="P12" t="s">
         <v>105</v>
       </c>
@@ -1377,6 +1411,9 @@
       </c>
       <c r="C13" t="s">
         <v>72</v>
+      </c>
+      <c r="O13" t="s">
+        <v>139</v>
       </c>
       <c r="P13" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
EPI-551: Validate survey question calculation and writeToField.fieldType (#4436)
* Validate survey question calculation and writeToField.fieldType

* Fix vitals name from a previous merge

* Turn on validateQuestionConfigs

* Don't make result calculations mandatory

* Disable validateQuestionConfigs by default
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkennedy/proj/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007E2631-B1FC-0744-9C1C-22F5E7293E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD773F57-6DD4-3043-BEE2-F8EF30773747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="-18740" windowWidth="33100" windowHeight="16440" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
   <si>
     <t>programName</t>
   </si>
@@ -454,7 +454,13 @@
     <t>test-questions-program</t>
   </si>
   <si>
-    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "def" } }</t>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>2+2</t>
+  </si>
+  <si>
+    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "FreeText" } }</t>
   </si>
 </sst>
 </file>
@@ -473,6 +479,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -937,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1034,6 +1041,9 @@
       <c r="K3" t="s">
         <v>131</v>
       </c>
+      <c r="O3" t="s">
+        <v>138</v>
+      </c>
       <c r="P3" t="s">
         <v>132</v>
       </c>
@@ -1051,6 +1061,9 @@
       <c r="K4" t="s">
         <v>131</v>
       </c>
+      <c r="O4" t="s">
+        <v>139</v>
+      </c>
       <c r="P4" t="s">
         <v>132</v>
       </c>
@@ -1066,7 +1079,7 @@
         <v>125</v>
       </c>
       <c r="P5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1148,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82512E0-EE41-F34F-B49B-D4799E578BC3}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1283,6 +1296,9 @@
       <c r="K6" t="s">
         <v>105</v>
       </c>
+      <c r="O6" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1297,6 +1313,9 @@
       <c r="K7" t="s">
         <v>106</v>
       </c>
+      <c r="O7" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1308,6 +1327,9 @@
       <c r="C8" t="s">
         <v>67</v>
       </c>
+      <c r="O8" t="s">
+        <v>138</v>
+      </c>
       <c r="P8" t="s">
         <v>105</v>
       </c>
@@ -1322,6 +1344,9 @@
       <c r="C9" t="s">
         <v>68</v>
       </c>
+      <c r="O9" t="s">
+        <v>139</v>
+      </c>
       <c r="P9" t="s">
         <v>107</v>
       </c>
@@ -1339,6 +1364,9 @@
       <c r="K10" t="s">
         <v>105</v>
       </c>
+      <c r="O10" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1353,6 +1381,9 @@
       <c r="K11" t="s">
         <v>106</v>
       </c>
+      <c r="O11" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1364,6 +1395,9 @@
       <c r="C12" t="s">
         <v>71</v>
       </c>
+      <c r="O12" t="s">
+        <v>138</v>
+      </c>
       <c r="P12" t="s">
         <v>105</v>
       </c>
@@ -1377,6 +1411,9 @@
       </c>
       <c r="C13" t="s">
         <v>72</v>
+      </c>
+      <c r="O13" t="s">
+        <v>139</v>
       </c>
       <c r="P13" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
Fix config validation test
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanmcquarrie/Documents/tamanu/packages/sync-server/__tests__/importers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alastair\BE\tamanu\packages\sync-server\__tests__\importers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007E2631-B1FC-0744-9C1C-22F5E7293E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37FFEBB-4FA5-4CE9-927E-29CBCB630EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="-18740" windowWidth="33100" windowHeight="16440" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
     <t>test-questions-program</t>
   </si>
   <si>
-    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "def" } }</t>
+    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc",  "fieldType": "def" } }</t>
   </si>
 </sst>
 </file>
@@ -473,6 +473,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -821,15 +822,15 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -845,7 +846,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -853,12 +854,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -881,7 +882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -904,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -937,24 +938,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.375" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="72.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="72.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="84.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="84.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -1083,7 +1084,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -1111,7 +1112,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -1125,7 +1126,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>121</v>
       </c>
@@ -1152,19 +1153,19 @@
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1228,7 +1229,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1242,7 +1243,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1298,7 +1299,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1326,7 +1327,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1340,7 +1341,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1354,7 +1355,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1382,7 +1383,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1396,7 +1397,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1424,7 +1425,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1466,7 +1467,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1480,7 +1481,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1494,7 +1495,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -1522,7 +1523,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1536,7 +1537,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -1550,7 +1551,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1592,7 +1593,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1606,7 +1607,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -1620,7 +1621,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Incorporate test xlsx changes from main
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alastair\BE\tamanu\packages\sync-server\__tests__\importers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\locke\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37FFEBB-4FA5-4CE9-927E-29CBCB630EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17927265-2FDD-43BE-A88D-9B8A318BB41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
+    <workbookView xWindow="-29055" yWindow="1155" windowWidth="25650" windowHeight="14250" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
   <si>
     <t>programName</t>
   </si>
@@ -454,7 +454,13 @@
     <t>test-questions-program</t>
   </si>
   <si>
-    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc",  "fieldType": "def" } }</t>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>2+2</t>
+  </si>
+  <si>
+    <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "fieldType": "FreeText" } }</t>
   </si>
 </sst>
 </file>
@@ -938,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1035,6 +1041,9 @@
       <c r="K3" t="s">
         <v>131</v>
       </c>
+      <c r="O3" t="s">
+        <v>138</v>
+      </c>
       <c r="P3" t="s">
         <v>132</v>
       </c>
@@ -1052,6 +1061,9 @@
       <c r="K4" t="s">
         <v>131</v>
       </c>
+      <c r="O4" t="s">
+        <v>139</v>
+      </c>
       <c r="P4" t="s">
         <v>132</v>
       </c>
@@ -1067,7 +1079,7 @@
         <v>125</v>
       </c>
       <c r="P5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1149,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82512E0-EE41-F34F-B49B-D4799E578BC3}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1284,6 +1296,9 @@
       <c r="K6" t="s">
         <v>105</v>
       </c>
+      <c r="O6" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1298,6 +1313,9 @@
       <c r="K7" t="s">
         <v>106</v>
       </c>
+      <c r="O7" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1309,6 +1327,9 @@
       <c r="C8" t="s">
         <v>67</v>
       </c>
+      <c r="O8" t="s">
+        <v>138</v>
+      </c>
       <c r="P8" t="s">
         <v>105</v>
       </c>
@@ -1323,6 +1344,9 @@
       <c r="C9" t="s">
         <v>68</v>
       </c>
+      <c r="O9" t="s">
+        <v>139</v>
+      </c>
       <c r="P9" t="s">
         <v>107</v>
       </c>
@@ -1340,6 +1364,9 @@
       <c r="K10" t="s">
         <v>105</v>
       </c>
+      <c r="O10" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1354,6 +1381,9 @@
       <c r="K11" t="s">
         <v>106</v>
       </c>
+      <c r="O11" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1365,6 +1395,9 @@
       <c r="C12" t="s">
         <v>71</v>
       </c>
+      <c r="O12" t="s">
+        <v>138</v>
+      </c>
       <c r="P12" t="s">
         <v>105</v>
       </c>
@@ -1378,6 +1411,9 @@
       </c>
       <c r="C13" t="s">
         <v>72</v>
+      </c>
+      <c r="O13" t="s">
+        <v>139</v>
       </c>
       <c r="P13" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
Add rows for mandatory test
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkennedy/proj/tamanu/packages/sync-server/__tests__/importers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biao/Documents/GitHub/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD773F57-6DD4-3043-BEE2-F8EF30773747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D2190-E2D3-8F4F-B1E8-B1101FA159F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="145">
   <si>
     <t>programName</t>
   </si>
@@ -461,6 +461,18 @@
   </si>
   <si>
     <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "FreeText" } }</t>
+  </si>
+  <si>
+    <t>Succeed-validationCriteria-mandatory-2</t>
+  </si>
+  <si>
+    <t>Succeed-validationCriteria-mandatory-1</t>
+  </si>
+  <si>
+    <t>{ "mandatory": {"encounterType":"admission"} }</t>
+  </si>
+  <si>
+    <t>{ "mandatory": {"encounterType":["admission","surveyResponse"]} }</t>
   </si>
 </sst>
 </file>
@@ -942,15 +954,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
@@ -1152,8 +1164,43 @@
         <v>135</v>
       </c>
     </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" t="s">
+        <v>143</v>
+      </c>
+      <c r="P11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" t="s">
+        <v>144</v>
+      </c>
+      <c r="P12" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1162,7 +1209,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
EPI-634 Vitals make vital field mandatory by encounter type (#4771)
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkennedy/proj/tamanu/packages/sync-server/__tests__/importers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biao/Documents/GitHub/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD773F57-6DD4-3043-BEE2-F8EF30773747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D2190-E2D3-8F4F-B1E8-B1101FA159F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="145">
   <si>
     <t>programName</t>
   </si>
@@ -461,6 +461,18 @@
   </si>
   <si>
     <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "FreeText" } }</t>
+  </si>
+  <si>
+    <t>Succeed-validationCriteria-mandatory-2</t>
+  </si>
+  <si>
+    <t>Succeed-validationCriteria-mandatory-1</t>
+  </si>
+  <si>
+    <t>{ "mandatory": {"encounterType":"admission"} }</t>
+  </si>
+  <si>
+    <t>{ "mandatory": {"encounterType":["admission","surveyResponse"]} }</t>
   </si>
 </sst>
 </file>
@@ -942,15 +954,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
@@ -1152,8 +1164,43 @@
         <v>135</v>
       </c>
     </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" t="s">
+        <v>143</v>
+      </c>
+      <c r="P11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" t="s">
+        <v>144</v>
+      </c>
+      <c r="P12" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1162,7 +1209,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
EPI-634 Make vital field mandatory by encounter type (#4762)
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
+++ b/packages/sync-server/__tests__/importers/programs-question-validation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkennedy/proj/tamanu/packages/sync-server/__tests__/importers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biao/Documents/GitHub/tamanu/packages/sync-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD773F57-6DD4-3043-BEE2-F8EF30773747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D2190-E2D3-8F4F-B1E8-B1101FA159F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{1DEB62B3-264E-1144-868E-C46669C3E049}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="145">
   <si>
     <t>programName</t>
   </si>
@@ -461,6 +461,18 @@
   </si>
   <si>
     <t>{ "column": "xyz", "writeToPatient": { "fieldName": "abc", "isAdditionalData": false, "fieldType": "FreeText" } }</t>
+  </si>
+  <si>
+    <t>Succeed-validationCriteria-mandatory-2</t>
+  </si>
+  <si>
+    <t>Succeed-validationCriteria-mandatory-1</t>
+  </si>
+  <si>
+    <t>{ "mandatory": {"encounterType":"admission"} }</t>
+  </si>
+  <si>
+    <t>{ "mandatory": {"encounterType":["admission","surveyResponse"]} }</t>
   </si>
 </sst>
 </file>
@@ -942,15 +954,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607E7730-B5CD-234F-B331-CA1E0A3F137F}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
@@ -1152,8 +1164,43 @@
         <v>135</v>
       </c>
     </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" t="s">
+        <v>143</v>
+      </c>
+      <c r="P11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" t="s">
+        <v>144</v>
+      </c>
+      <c r="P12" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1162,7 +1209,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>